<commit_message>
UPFDATED THE TEST CASES FILE
</commit_message>
<xml_diff>
--- a/03Test Scenario Design/TEST_SCENARIO.xlsx
+++ b/03Test Scenario Design/TEST_SCENARIO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\SOFTWARE TESTING\TESTING PROJECTS\Opencart.demo testing project\03Test Scenario Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41DD47B-5FBA-48E1-B204-3F580968DD12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6205C0-1DAA-43B6-889C-80AD0791EE79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -491,7 +491,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
UPDATED TEST CASE FILE WITH ALL FIELDS
</commit_message>
<xml_diff>
--- a/03Test Scenario Design/TEST_SCENARIO.xlsx
+++ b/03Test Scenario Design/TEST_SCENARIO.xlsx
@@ -8,17 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\SOFTWARE TESTING\TESTING PROJECTS\Opencart.demo testing project\03Test Scenario Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6205C0-1DAA-43B6-889C-80AD0791EE79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD829CD1-1614-44A1-96E8-21FD0BBC1713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10560" yWindow="345" windowWidth="10275" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -490,15 +499,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
     <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -507,10 +516,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
@@ -521,10 +530,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
@@ -535,10 +544,10 @@
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -549,10 +558,10 @@
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>7</v>
@@ -563,24 +572,24 @@
         <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>19</v>
@@ -591,10 +600,10 @@
         <v>20</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>7</v>
@@ -605,10 +614,10 @@
         <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>19</v>
@@ -619,10 +628,10 @@
         <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>19</v>
@@ -633,10 +642,10 @@
         <v>27</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>7</v>
@@ -647,10 +656,10 @@
         <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>7</v>
@@ -661,10 +670,10 @@
         <v>32</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>7</v>
@@ -675,10 +684,10 @@
         <v>34</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>19</v>
@@ -689,10 +698,10 @@
         <v>37</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>19</v>
@@ -703,10 +712,10 @@
         <v>40</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>19</v>

</xml_diff>